<commit_message>
add timeline to  easy follow this project
</commit_message>
<xml_diff>
--- a/cra-ecommerce/BackLog.xlsx
+++ b/cra-ecommerce/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\SelfLearning\PersonalProject\EcommerceManage\cra-ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0D7F12-BE46-4D12-AB74-2855FEA24013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293589A8-E984-453A-8E09-084937E6CD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
   <si>
     <t>E-COMMERCE PROJECT - PRODUCT BACKLOG</t>
   </si>
@@ -320,6 +320,24 @@
     <t>(deleteCategory in blogCategory) Admin xóa bằng id danh mục sp và token admin</t>
   </si>
   <si>
+    <t xml:space="preserve">Xem danh mục diễn đàn trên sàn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (getCategory in productCategory) Mọi đối tượng</t>
+  </si>
+  <si>
+    <t>(getCategory in blogCategory) Mọi đối tượng</t>
+  </si>
+  <si>
+    <t>Xóa bằng id account Admin đó</t>
+  </si>
+  <si>
+    <t>Tạo tài khoản admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tài khoản của admin chỉ được đăng kí bởi 1 tài khoản admin đã có sẵn trước đó </t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">(creatCategory in blogCategory) Admin có thể tạo hoặc tạo theo mong muốn từ người bán 
 </t>
@@ -343,17 +361,33 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> : 1.1 Tết siêu sale ,25.12 Cuối năm sắm sửa ,....</t>
+      <t xml:space="preserve"> : 1.1 Tết siêu sale ,25.12 Cuối năm sắm sửa ,....
+Diễn đàn bao gồm : tựa đề, mô tả, mã giảm giá, danh mục diễn đàn, </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Xem danh mục diễn đàn trên sàn </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (getCategory in productCategory) Mọi đối tượng</t>
-  </si>
-  <si>
-    <t>(getCategory in blogCategory) Mọi đối tượng</t>
+    <t>Tạo diễn đàn</t>
+  </si>
+  <si>
+    <t>Sửa thông tin diễn đàn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(createNewBlog in Blog) Diễn đàn bao gồm những thông tin : Tên (title) ,mô tả, mã giảm giá(coupon), danh mục diễn đàn, </t>
+  </si>
+  <si>
+    <t>Xóa diễn đàn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(deleteBlog in Blog) Admin xóa bằng _id của diễn đàn </t>
+  </si>
+  <si>
+    <t>(updateBlog in Blog) Admin cần phải cung cấp bearer token và id của blogs để update</t>
+  </si>
+  <si>
+    <t>Xem diễn đàn</t>
+  </si>
+  <si>
+    <t>(getBlogs in Blog) Mọi đối tượng</t>
   </si>
 </sst>
 </file>
@@ -482,12 +516,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,11 +802,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -785,13 +819,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -821,18 +855,18 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6">
-        <f>SUM(C6:C46)</f>
+        <f>SUM(C6:C51)</f>
         <v>34</v>
       </c>
       <c r="D4" s="6">
-        <f>SUM(D6:D46)</f>
+        <f>SUM(D6:D51)</f>
         <v>10</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1"/>
@@ -987,7 +1021,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -995,147 +1029,151 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.4">
+      <c r="A18" s="7"/>
+      <c r="B18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
         <v>9</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C19" s="6">
         <v>4</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D19" s="6">
         <v>2</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
+    <row r="20" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="6">
         <v>10</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C20" s="6">
         <v>2</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="10" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="10" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
-        <v>11</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
         <v>13</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
-        <v>14</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="25" x14ac:dyDescent="0.5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="15" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>14</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="25" x14ac:dyDescent="0.5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6">
         <v>15</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
-        <v>16</v>
-      </c>
       <c r="B26" s="11" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="3" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
+      <c r="A27" s="6">
+        <v>15</v>
+      </c>
       <c r="B27" s="11" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
+      <c r="A28" s="6">
+        <v>16</v>
+      </c>
       <c r="B28" s="11" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1144,305 +1182,325 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
-        <v>17</v>
-      </c>
+      <c r="A29" s="6"/>
       <c r="B29" s="11" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="11" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
+      <c r="E30" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="6">
+        <v>17</v>
+      </c>
       <c r="B31" s="11" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
-      <c r="B33" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="6">
-        <v>2</v>
-      </c>
+      <c r="B33" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
-      <c r="B34" s="8" t="s">
-        <v>44</v>
+      <c r="B34" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="C35" s="6">
+        <v>2</v>
+      </c>
       <c r="D35" s="6"/>
       <c r="E35" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A40" s="1"/>
-      <c r="B40" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A41" s="6">
-        <v>18</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="6"/>
+      <c r="B40" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="6"/>
       <c r="B41" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="6">
-        <v>3</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="6">
-        <v>19</v>
-      </c>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="6"/>
       <c r="B42" s="8" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="3"/>
+      <c r="E42" s="10" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="6">
-        <v>20</v>
-      </c>
+      <c r="A43" s="6"/>
       <c r="B43" s="8" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="6">
-        <v>21</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>18</v>
+      <c r="E43" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="6"/>
+      <c r="B44" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="6">
-        <v>22</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E44" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.4">
+      <c r="A45" s="1"/>
+      <c r="B45" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C46" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="C46" s="6">
+        <v>3</v>
+      </c>
       <c r="D46" s="6"/>
       <c r="E46" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="6">
+        <v>19</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="6">
+        <v>20</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="6">
+        <v>21</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="6">
+        <v>22</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="6">
+        <v>23</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="10" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="3"/>
-      <c r="B47" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="3"/>
-      <c r="B48" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="3"/>
-      <c r="B49" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
-      <c r="B52" s="3" t="s">
-        <v>59</v>
+      <c r="B52" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
+      <c r="B53" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
+      <c r="B54" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
+      <c r="B55" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
+      <c r="B56" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
+      <c r="B57" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
@@ -1660,6 +1718,41 @@
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
CRUD coupon :phiếu mua hàng /giảm giá
</commit_message>
<xml_diff>
--- a/cra-ecommerce/BackLog.xlsx
+++ b/cra-ecommerce/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\SelfLearning\PersonalProject\EcommerceManage\cra-ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD84A021-66AB-4DB8-A75D-4E1DF2AE4FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3020B4-BAC8-409B-A962-3FB2B333F4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
   <si>
     <t>E-COMMERCE PROJECT - PRODUCT BACKLOG</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>(getBrands in Brand) Mọi đối tượng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tạo phíếu mua hàng </t>
   </si>
 </sst>
 </file>
@@ -864,11 +867,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,11 +920,11 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6">
-        <f>SUM(C6:C56)</f>
+        <f>SUM(C6:C57)</f>
         <v>34</v>
       </c>
       <c r="D4" s="6">
-        <f>SUM(D6:D56)</f>
+        <f>SUM(D6:D57)</f>
         <v>10</v>
       </c>
       <c r="E4" s="3"/>
@@ -1476,179 +1479,181 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A50" s="1"/>
-      <c r="B50" s="13" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="6"/>
+      <c r="B50" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.4">
+      <c r="A51" s="1"/>
+      <c r="B51" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="51" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A51" s="6">
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="7"/>
+    </row>
+    <row r="52" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A52" s="6">
         <v>18</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B52" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C52" s="6">
         <v>3</v>
       </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="10" t="s">
+      <c r="D52" s="6"/>
+      <c r="E52" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="6">
-        <v>19</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
-      <c r="E53" s="10"/>
-    </row>
-    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
-        <v>21</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
-      <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
-        <v>22</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
-      <c r="E56" s="10" t="s">
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="6">
+        <v>23</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="3"/>
-      <c r="B57" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
-      <c r="E58" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="E58" s="3"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="3"/>
-      <c r="B60" s="3" t="s">
-        <v>45</v>
+      <c r="B60" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
       <c r="B63" s="3" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
       <c r="B64" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
+      <c r="B65" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="3"/>
@@ -1880,6 +1885,13 @@
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>